<commit_message>
Ajout liens classes aad360e5fee5029c63105e72d3ce4f0f9c39d95f
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/StructureDefinition-ExerciceProfessionnel.xlsx
+++ b/poc-professionnel/ig/StructureDefinition-ExerciceProfessionnel.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="150">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-24T12:59:21+00:00</t>
+    <t>2025-07-24T13:17:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -461,6 +461,16 @@
   </si>
   <si>
     <t>Date à laquelle le niveau de formation n’est plus actif (non visible hormis dans les données historisées). Cette date est renseignée par l’ordre à la clôture de l’exercice professionnel.</t>
+  </si>
+  <si>
+    <t>ExerciceProfessionnel.professionnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/mos/StructureDefinition/Professionnel)
+</t>
+  </si>
+  <si>
+    <t>Lien vers la classe Professionnel.</t>
   </si>
 </sst>
 </file>
@@ -763,7 +773,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ28"/>
+  <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -782,7 +792,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="61.14453125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="68.80078125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -3595,6 +3605,106 @@
         <v>70</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="G29" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="I29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="J29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="Q29" s="2"/>
+      <c r="R29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="S29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="T29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="U29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="V29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="W29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>